<commit_message>
Multi sheet importer (parser) v.0.92.
</commit_message>
<xml_diff>
--- a/src/test/resources/Test_chain_products.xlsx
+++ b/src/test/resources/Test_chain_products.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="36">
   <si>
     <t>Наименование</t>
   </si>
@@ -41,12 +41,6 @@
     <t>Цена до акции</t>
   </si>
   <si>
-    <t>КГ</t>
-  </si>
-  <si>
-    <t>ШТ</t>
-  </si>
-  <si>
     <t>Штрих-код</t>
   </si>
   <si>
@@ -125,84 +119,6 @@
     <t>Z040</t>
   </si>
   <si>
-    <t>П/ф смесь мучная Оладьи по домашнему 500г Шт</t>
-  </si>
-  <si>
-    <t>П/ф смесь мучная Пицца 500г Шт</t>
-  </si>
-  <si>
-    <t>Козинак из арахиса 170г Шт</t>
-  </si>
-  <si>
-    <t>Резинка жевательная Orbit сладкая мята 13,6г Шт</t>
-  </si>
-  <si>
-    <t>Кофе молотый Lavazza мол qualita rossa int 250г ж/б Шт</t>
-  </si>
-  <si>
-    <t>Изделия макаронные Gallina blanca Спагетти 450г Шт</t>
-  </si>
-  <si>
-    <t>Сосиски м/пт Мишутка с сыром в/с 480г фас Шт</t>
-  </si>
-  <si>
-    <t>Пельмени Vici с курицей оригинальные 400г Шт</t>
-  </si>
-  <si>
-    <t>Корм конс для взр собак Chappi сытн мясн обед курочка аппет 100г Шт</t>
-  </si>
-  <si>
-    <t>Корм конс для взр собак Chappi сытн мясн обед с говяд по-домаш 100г Шт</t>
-  </si>
-  <si>
-    <t>СТОЛИЧНАЯ МЕЛЬНИЦА</t>
-  </si>
-  <si>
-    <t>АЗОВСКАЯ КОНДИТЕРСКАЯ ФАБРИКА</t>
-  </si>
-  <si>
-    <t>ORBIT</t>
-  </si>
-  <si>
-    <t>LAVAZZA</t>
-  </si>
-  <si>
-    <t>GALLINA BLANCA</t>
-  </si>
-  <si>
-    <t>БРАТЬЯ ГРИЛЛЬ</t>
-  </si>
-  <si>
-    <t>CHAPPI</t>
-  </si>
-  <si>
-    <t>Азовская кондитерская фабрика</t>
-  </si>
-  <si>
-    <t>Wrigley GmbH</t>
-  </si>
-  <si>
-    <t>Лавацца</t>
-  </si>
-  <si>
-    <t>Юроп Фудс ГБ</t>
-  </si>
-  <si>
-    <t>Серволюкс Агро филиал Белмит</t>
-  </si>
-  <si>
-    <t>Марс</t>
-  </si>
-  <si>
-    <t>BY</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>LT</t>
-  </si>
-  <si>
     <t>ВидРеклМероприятия</t>
   </si>
   <si>
@@ -213,6 +129,12 @@
   </si>
   <si>
     <t>КодСтраны</t>
+  </si>
+  <si>
+    <t>кг</t>
+  </si>
+  <si>
+    <t>шт</t>
   </si>
 </sst>
 </file>
@@ -263,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -287,12 +209,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -575,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,7 +512,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -608,36 +524,36 @@
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D2" s="6">
         <v>3.19</v>
@@ -660,13 +576,13 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D3" s="6">
         <v>2.39</v>
@@ -684,24 +600,24 @@
         <v>4607037121607</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D4" s="6">
         <v>1.65</v>
@@ -719,24 +635,24 @@
         <v>4770190038461</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D5" s="6">
         <v>1.99</v>
@@ -754,24 +670,24 @@
         <v>4740056095082</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D6" s="6">
         <v>0.59</v>
@@ -789,24 +705,24 @@
         <v>8722700343486</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K6" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D7" s="6">
         <v>4.3899999999999997</v>
@@ -824,24 +740,24 @@
         <v>4607029348166</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="D8" s="6">
         <v>3.99</v>
@@ -859,24 +775,24 @@
         <v>4791045003182</v>
       </c>
       <c r="I8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D9" s="6">
         <v>2.89</v>
@@ -899,13 +815,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D10" s="6">
         <v>3.39</v>
@@ -928,13 +844,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>4</v>
+        <v>34</v>
       </c>
       <c r="D11" s="6">
         <v>4.09</v>
@@ -954,353 +870,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12" s="9">
-        <v>1.39</v>
-      </c>
-      <c r="E12" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F12" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G12" s="9">
-        <v>1.85</v>
-      </c>
-      <c r="H12" s="10">
-        <v>4810047000743</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="9">
-        <v>1.05</v>
-      </c>
-      <c r="E13" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F13" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G13" s="9">
-        <v>1.42</v>
-      </c>
-      <c r="H13" s="10">
-        <v>4810047000774</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="9">
-        <v>1.69</v>
-      </c>
-      <c r="E14" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F14" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G14" s="9">
-        <v>2.19</v>
-      </c>
-      <c r="H14" s="10">
-        <v>4620004251220</v>
-      </c>
-      <c r="I14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="9">
-        <v>0.71</v>
-      </c>
-      <c r="E15" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F15" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G15" s="9">
-        <v>0.88</v>
-      </c>
-      <c r="H15" s="10">
-        <v>50173808</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="K15" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16" s="9">
-        <v>13.59</v>
-      </c>
-      <c r="E16" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F16" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G16" s="9">
-        <v>17.989999999999998</v>
-      </c>
-      <c r="H16" s="10">
-        <v>8000070035935</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="9">
-        <v>1.75</v>
-      </c>
-      <c r="E17" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F17" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G17" s="9">
-        <v>2.59</v>
-      </c>
-      <c r="H17" s="10">
-        <v>8410300236610</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K17" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="9">
-        <v>3.99</v>
-      </c>
-      <c r="E18" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F18" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G18" s="9">
-        <v>5.05</v>
-      </c>
-      <c r="H18" s="10">
-        <v>4810953019495</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="9">
-        <v>3.79</v>
-      </c>
-      <c r="E19" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F19" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G19" s="9">
-        <v>4.99</v>
-      </c>
-      <c r="H19" s="10">
-        <v>4770190077828</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20" s="9">
-        <v>0.45</v>
-      </c>
-      <c r="E20" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F20" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G20" s="9">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="H20" s="10">
-        <v>4607065002848</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K20" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" s="9">
-        <v>0.45</v>
-      </c>
-      <c r="E21" s="7">
-        <v>43426</v>
-      </c>
-      <c r="F21" s="7">
-        <v>43797</v>
-      </c>
-      <c r="G21" s="9">
-        <v>0.56999999999999995</v>
-      </c>
-      <c r="H21" s="10">
-        <v>4607065002862</v>
-      </c>
-      <c r="I21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>